<commit_message>
updated navigator and started on-board simulator node
</commit_message>
<xml_diff>
--- a/Power Budget.xlsx
+++ b/Power Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/502ffe03a760cb01/Documents/PiQuad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/502ffe03a760cb01/Documents/PiQuad/PiCopter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{BCBB156B-6718-4A6F-A858-FAB2EFBB5CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C12E9939-846E-4D4B-8D98-4824CFB3C210}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{BCBB156B-6718-4A6F-A858-FAB2EFBB5CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC9DC241-4A68-43CF-98B5-D350A170231F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{244017E7-A73F-481C-8F2A-BCA50FCCEA61}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{244017E7-A73F-481C-8F2A-BCA50FCCEA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Component</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>14.8V 1500mAh</t>
+  </si>
+  <si>
+    <t>VL53L1X Distance Sensor</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +162,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +480,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +515,7 @@
       </c>
       <c r="B3" s="7">
         <f>(B2/E22)*60</f>
-        <v>3.5087719298245612</v>
+        <v>13.330371028660299</v>
       </c>
       <c r="C3" s="9"/>
     </row>
@@ -573,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="3">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3">
         <v>4</v>
@@ -583,7 +587,7 @@
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -605,13 +609,21 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -724,22 +736,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="5">
         <f>SUM(B6:B21)</f>
-        <v>93</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
+        <v>30.02</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5">
         <f t="shared" ref="D22:E22" si="1">SUM(D6:D21)</f>
-        <v>4</v>
-      </c>
-      <c r="E22" s="3">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5">
         <f t="shared" si="1"/>
-        <v>342</v>
+        <v>90.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>